<commit_message>
Changed sql and xlsx file for testing
</commit_message>
<xml_diff>
--- a/exc1.xlsx
+++ b/exc1.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Initialized textzss</t>
+    <t>Initialized text</t>
+  </si>
+  <si>
+    <t>This is new, can git see me?</t>
   </si>
 </sst>
 </file>
@@ -29,7 +32,7 @@
     <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,44 +43,45 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,11 +95,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,6 +125,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -131,59 +141,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,25 +194,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,25 +308,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,13 +344,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,103 +374,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,6 +385,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -403,15 +408,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -434,8 +430,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -443,8 +439,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,148 +488,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -958,17 +954,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>